<commit_message>
Fixed reading ordered date and read tracking number field
</commit_message>
<xml_diff>
--- a/ApplicationCore/ApplicationCore.Tests.Unit/HafeleMDFDoorOrderLoading/TestData/Test1.3.xlsx
+++ b/ApplicationCore/ApplicationCore.Tests.Unit/HafeleMDFDoorOrderLoading/TestData/Test1.3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\Door Orders\Hafele\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zachary Londono\source\repos\OrderProcessor\ApplicationCore\ApplicationCore.Tests.Unit\HafeleMDFDoorOrderLoading\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7D8A362-82A4-4F39-A18B-8E165227C849}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE49F101-98DF-4AA2-8169-755BECC13C89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{055880C2-27AA-406A-A981-7BEBAEB91D4D}"/>
+    <workbookView xWindow="11985" yWindow="1185" windowWidth="15255" windowHeight="13650" xr2:uid="{055880C2-27AA-406A-A981-7BEBAEB91D4D}"/>
   </bookViews>
   <sheets>
     <sheet name="Options" sheetId="3" r:id="rId1"/>
@@ -132,7 +132,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -162,7 +161,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="176">
   <si>
     <t>Qty</t>
   </si>
@@ -700,6 +699,9 @@
   </si>
   <si>
     <t>HafeleOrderNum</t>
+  </si>
+  <si>
+    <t>Tracking Number</t>
   </si>
 </sst>
 </file>
@@ -1286,27 +1288,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
@@ -1319,7 +1300,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1359,6 +1346,21 @@
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1547,7 +1549,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="Framing_Bead_Image" spid="_x0000_s1879"/>
+                  <a14:cameraTool cellRange="Framing_Bead_Image" spid="_x0000_s1889"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -1635,7 +1637,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="Edge_Profile_Image" spid="_x0000_s1880"/>
+                  <a14:cameraTool cellRange="Edge_Profile_Image" spid="_x0000_s1890"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -1723,7 +1725,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="Panel_Detail_Image" spid="_x0000_s1881"/>
+                  <a14:cameraTool cellRange="Panel_Detail_Image" spid="_x0000_s1891"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -3854,10 +3856,10 @@
   <sheetData>
     <row r="1" spans="2:8" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:8" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G2" s="51" t="s">
+      <c r="G2" s="53" t="s">
         <v>71</v>
       </c>
-      <c r="H2" s="52"/>
+      <c r="H2" s="55"/>
     </row>
     <row r="3" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="G3" s="5" t="s">
@@ -3884,13 +3886,13 @@
       </c>
     </row>
     <row r="6" spans="2:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="53" t="str" cm="1">
+      <c r="B6" s="71" t="str" cm="1">
         <f t="array" ref="B6">"MDF Door Configurator      " &amp; WBVersion</f>
         <v>MDF Door Configurator      Beta 1.3</v>
       </c>
-      <c r="C6" s="53"/>
-      <c r="D6" s="53"/>
-      <c r="E6" s="53"/>
+      <c r="C6" s="71"/>
+      <c r="D6" s="71"/>
+      <c r="E6" s="71"/>
       <c r="G6" s="12" t="s">
         <v>39</v>
       </c>
@@ -3900,10 +3902,10 @@
     </row>
     <row r="7" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C8" s="49" t="s">
+      <c r="C8" s="69" t="s">
         <v>97</v>
       </c>
-      <c r="D8" s="50"/>
+      <c r="D8" s="70"/>
       <c r="G8" s="5" t="s">
         <v>41</v>
       </c>
@@ -3937,22 +3939,22 @@
     </row>
     <row r="11" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="2:8" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="51" t="s">
+      <c r="B12" s="53" t="s">
         <v>74</v>
       </c>
-      <c r="C12" s="60"/>
-      <c r="D12" s="60"/>
-      <c r="E12" s="52"/>
-      <c r="G12" s="51" t="s">
+      <c r="C12" s="54"/>
+      <c r="D12" s="54"/>
+      <c r="E12" s="55"/>
+      <c r="G12" s="53" t="s">
         <v>72</v>
       </c>
-      <c r="H12" s="52"/>
+      <c r="H12" s="55"/>
     </row>
     <row r="13" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B13" s="61"/>
-      <c r="C13" s="62"/>
-      <c r="D13" s="62"/>
-      <c r="E13" s="63"/>
+      <c r="B13" s="56"/>
+      <c r="C13" s="57"/>
+      <c r="D13" s="57"/>
+      <c r="E13" s="58"/>
       <c r="G13" s="5" t="s">
         <v>139</v>
       </c>
@@ -3961,10 +3963,10 @@
       </c>
     </row>
     <row r="14" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="64"/>
-      <c r="C14" s="65"/>
-      <c r="D14" s="65"/>
-      <c r="E14" s="66"/>
+      <c r="B14" s="59"/>
+      <c r="C14" s="60"/>
+      <c r="D14" s="60"/>
+      <c r="E14" s="61"/>
       <c r="G14" s="24" t="s">
         <v>136</v>
       </c>
@@ -3973,10 +3975,10 @@
       </c>
     </row>
     <row r="15" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B15" s="64"/>
-      <c r="C15" s="65"/>
-      <c r="D15" s="65"/>
-      <c r="E15" s="66"/>
+      <c r="B15" s="59"/>
+      <c r="C15" s="60"/>
+      <c r="D15" s="60"/>
+      <c r="E15" s="61"/>
       <c r="G15" s="6" t="s">
         <v>140</v>
       </c>
@@ -3986,10 +3988,10 @@
       </c>
     </row>
     <row r="16" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="64"/>
-      <c r="C16" s="65"/>
-      <c r="D16" s="65"/>
-      <c r="E16" s="66"/>
+      <c r="B16" s="59"/>
+      <c r="C16" s="60"/>
+      <c r="D16" s="60"/>
+      <c r="E16" s="61"/>
       <c r="G16" s="6" t="s">
         <v>141</v>
       </c>
@@ -3999,10 +4001,10 @@
       </c>
     </row>
     <row r="17" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B17" s="64"/>
-      <c r="C17" s="65"/>
-      <c r="D17" s="65"/>
-      <c r="E17" s="66"/>
+      <c r="B17" s="59"/>
+      <c r="C17" s="60"/>
+      <c r="D17" s="60"/>
+      <c r="E17" s="61"/>
       <c r="G17" s="24" t="s">
         <v>137</v>
       </c>
@@ -4011,10 +4013,10 @@
       </c>
     </row>
     <row r="18" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B18" s="64"/>
-      <c r="C18" s="65"/>
-      <c r="D18" s="65"/>
-      <c r="E18" s="66"/>
+      <c r="B18" s="59"/>
+      <c r="C18" s="60"/>
+      <c r="D18" s="60"/>
+      <c r="E18" s="61"/>
       <c r="G18" s="6" t="s">
         <v>138</v>
       </c>
@@ -4023,10 +4025,10 @@
       </c>
     </row>
     <row r="19" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="67"/>
-      <c r="C19" s="68"/>
-      <c r="D19" s="68"/>
-      <c r="E19" s="69"/>
+      <c r="B19" s="62"/>
+      <c r="C19" s="63"/>
+      <c r="D19" s="63"/>
+      <c r="E19" s="64"/>
       <c r="G19" s="6" t="s">
         <v>132</v>
       </c>
@@ -4070,12 +4072,12 @@
     <row r="23" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="24" spans="2:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="25" spans="2:8" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="51" t="s">
+      <c r="B25" s="53" t="s">
         <v>75</v>
       </c>
-      <c r="C25" s="60"/>
-      <c r="D25" s="60"/>
-      <c r="E25" s="52"/>
+      <c r="C25" s="54"/>
+      <c r="D25" s="54"/>
+      <c r="E25" s="55"/>
       <c r="G25" s="42"/>
       <c r="H25" s="43"/>
     </row>
@@ -4083,9 +4085,11 @@
       <c r="B26" s="39" t="s">
         <v>76</v>
       </c>
-      <c r="C26" s="54"/>
-      <c r="D26" s="54"/>
-      <c r="E26" s="55"/>
+      <c r="C26" s="72" t="s">
+        <v>76</v>
+      </c>
+      <c r="D26" s="72"/>
+      <c r="E26" s="73"/>
       <c r="G26" s="8"/>
       <c r="H26" s="9"/>
     </row>
@@ -4093,9 +4097,11 @@
       <c r="B27" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="C27" s="70"/>
-      <c r="D27" s="70"/>
-      <c r="E27" s="71"/>
+      <c r="C27" s="65" t="s">
+        <v>36</v>
+      </c>
+      <c r="D27" s="65"/>
+      <c r="E27" s="66"/>
       <c r="G27" s="8"/>
       <c r="H27" s="9"/>
     </row>
@@ -4103,9 +4109,11 @@
       <c r="B28" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="C28" s="70"/>
-      <c r="D28" s="70"/>
-      <c r="E28" s="71"/>
+      <c r="C28" s="65" t="s">
+        <v>37</v>
+      </c>
+      <c r="D28" s="65"/>
+      <c r="E28" s="66"/>
       <c r="G28" s="8"/>
       <c r="H28" s="9"/>
     </row>
@@ -4113,9 +4121,11 @@
       <c r="B29" s="39" t="s">
         <v>77</v>
       </c>
-      <c r="C29" s="70"/>
-      <c r="D29" s="70"/>
-      <c r="E29" s="71"/>
+      <c r="C29" s="65" t="s">
+        <v>77</v>
+      </c>
+      <c r="D29" s="65"/>
+      <c r="E29" s="66"/>
       <c r="G29" s="8"/>
       <c r="H29" s="9"/>
     </row>
@@ -4123,9 +4133,11 @@
       <c r="B30" s="39" t="s">
         <v>78</v>
       </c>
-      <c r="C30" s="70"/>
-      <c r="D30" s="70"/>
-      <c r="E30" s="71"/>
+      <c r="C30" s="65" t="s">
+        <v>78</v>
+      </c>
+      <c r="D30" s="65"/>
+      <c r="E30" s="66"/>
       <c r="G30" s="8"/>
       <c r="H30" s="9"/>
     </row>
@@ -4133,9 +4145,11 @@
       <c r="B31" s="39" t="s">
         <v>79</v>
       </c>
-      <c r="C31" s="70"/>
-      <c r="D31" s="70"/>
-      <c r="E31" s="71"/>
+      <c r="C31" s="65" t="s">
+        <v>79</v>
+      </c>
+      <c r="D31" s="65"/>
+      <c r="E31" s="66"/>
       <c r="G31" s="10"/>
       <c r="H31" s="11"/>
     </row>
@@ -4143,9 +4157,11 @@
       <c r="B32" s="39" t="s">
         <v>80</v>
       </c>
-      <c r="C32" s="70"/>
-      <c r="D32" s="70"/>
-      <c r="E32" s="71"/>
+      <c r="C32" s="65" t="s">
+        <v>80</v>
+      </c>
+      <c r="D32" s="65"/>
+      <c r="E32" s="66"/>
       <c r="G32" s="8"/>
       <c r="H32" s="9"/>
     </row>
@@ -4153,9 +4169,11 @@
       <c r="B33" s="39" t="s">
         <v>81</v>
       </c>
-      <c r="C33" s="56"/>
-      <c r="D33" s="56"/>
-      <c r="E33" s="57"/>
+      <c r="C33" s="49" t="s">
+        <v>81</v>
+      </c>
+      <c r="D33" s="49"/>
+      <c r="E33" s="50"/>
       <c r="G33" s="8"/>
       <c r="H33" s="9"/>
     </row>
@@ -4163,9 +4181,11 @@
       <c r="B34" s="39" t="s">
         <v>82</v>
       </c>
-      <c r="C34" s="72"/>
-      <c r="D34" s="72"/>
-      <c r="E34" s="73"/>
+      <c r="C34" s="67" t="s">
+        <v>82</v>
+      </c>
+      <c r="D34" s="67"/>
+      <c r="E34" s="68"/>
       <c r="G34" s="8"/>
       <c r="H34" s="9"/>
     </row>
@@ -4173,9 +4193,11 @@
       <c r="B35" s="39" t="s">
         <v>83</v>
       </c>
-      <c r="C35" s="56"/>
-      <c r="D35" s="56"/>
-      <c r="E35" s="57"/>
+      <c r="C35" s="49" t="s">
+        <v>83</v>
+      </c>
+      <c r="D35" s="49"/>
+      <c r="E35" s="50"/>
       <c r="G35" s="8"/>
       <c r="H35" s="9"/>
     </row>
@@ -4183,11 +4205,11 @@
       <c r="B36" s="39" t="s">
         <v>84</v>
       </c>
-      <c r="C36" s="56" t="s">
+      <c r="C36" s="49" t="s">
         <v>112</v>
       </c>
-      <c r="D36" s="56"/>
-      <c r="E36" s="57"/>
+      <c r="D36" s="49"/>
+      <c r="E36" s="50"/>
       <c r="G36" s="8"/>
       <c r="H36" s="9"/>
     </row>
@@ -4195,9 +4217,11 @@
       <c r="B37" s="40" t="s">
         <v>169</v>
       </c>
-      <c r="C37" s="58"/>
-      <c r="D37" s="58"/>
-      <c r="E37" s="59"/>
+      <c r="C37" s="51" t="s">
+        <v>175</v>
+      </c>
+      <c r="D37" s="51"/>
+      <c r="E37" s="52"/>
       <c r="G37" s="8"/>
       <c r="H37" s="9"/>
     </row>
@@ -4235,6 +4259,11 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="C26:E26"/>
     <mergeCell ref="C36:E36"/>
     <mergeCell ref="C37:E37"/>
     <mergeCell ref="B25:E25"/>
@@ -4249,11 +4278,6 @@
     <mergeCell ref="C33:E33"/>
     <mergeCell ref="C34:E34"/>
     <mergeCell ref="C35:E35"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="C26:E26"/>
   </mergeCells>
   <conditionalFormatting sqref="G20:H20">
     <cfRule type="expression" dxfId="11" priority="1">

</xml_diff>